<commit_message>
Update examples and datasets
</commit_message>
<xml_diff>
--- a/data-raw/citypop.xlsx
+++ b/data-raw/citypop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolo/Library/CloudStorage/iCloud Drive/Documents/github/usmap/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D674697-3185-6345-AFDB-54A5202D9AA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45DB4AE-6408-364C-BD95-6C2812F2CE86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{1213CEC5-0E42-FB4F-8CDE-D4349F2F248A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="citypop" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">citypop!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">citypop!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="156">
   <si>
     <t>lon</t>
   </si>
@@ -345,6 +345,162 @@
   </si>
   <si>
     <t>Cheyenne</t>
+  </si>
+  <si>
+    <t>abbr</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WY</t>
   </si>
 </sst>
 </file>
@@ -705,7 +861,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C824B7D4-AA41-414F-8156-3522E009C776}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -714,7 +870,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,13 +881,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-86.81</v>
       </c>
@@ -742,13 +901,16 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>212237</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-149.9</v>
       </c>
@@ -759,13 +921,16 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>291826</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-112.07</v>
       </c>
@@ -776,13 +941,16 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1445632</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-92.33</v>
       </c>
@@ -793,13 +961,16 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>193524</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-118.25</v>
       </c>
@@ -810,13 +981,16 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3792621</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-104.88</v>
       </c>
@@ -827,13 +1001,16 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>600158</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-73.2</v>
       </c>
@@ -844,13 +1021,16 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>144229</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-75.55</v>
       </c>
@@ -861,13 +1041,16 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>70851</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-77.02</v>
       </c>
@@ -878,13 +1061,16 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>693972</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-81.66</v>
       </c>
@@ -895,13 +1081,16 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>880619</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-84.39</v>
       </c>
@@ -912,13 +1101,16 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>420003</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-157.82</v>
       </c>
@@ -929,13 +1121,16 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="s">
         <v>28</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>337256</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-116.2</v>
       </c>
@@ -946,13 +1141,16 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>205671</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-87.63</v>
       </c>
@@ -963,13 +1161,16 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
         <v>32</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>2695598</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-86.16</v>
       </c>
@@ -980,13 +1181,16 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>820445</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-93.62</v>
       </c>
@@ -997,13 +1201,16 @@
         <v>35</v>
       </c>
       <c r="D17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>215472</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-97.34</v>
       </c>
@@ -1014,13 +1221,16 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" t="s">
         <v>38</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>382368</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-85.74</v>
       </c>
@@ -1031,13 +1241,16 @@
         <v>39</v>
       </c>
       <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
         <v>40</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>597337</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-90.08</v>
       </c>
@@ -1048,13 +1261,16 @@
         <v>41</v>
       </c>
       <c r="D20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" t="s">
         <v>42</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>343829</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-70.27</v>
       </c>
@@ -1065,13 +1281,16 @@
         <v>43</v>
       </c>
       <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" t="s">
         <v>44</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>66194</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-76.62</v>
       </c>
@@ -1082,13 +1301,16 @@
         <v>45</v>
       </c>
       <c r="D22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" t="s">
         <v>46</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>620961</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-71.06</v>
       </c>
@@ -1099,13 +1321,16 @@
         <v>47</v>
       </c>
       <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" t="s">
         <v>48</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>617594</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-83.05</v>
       </c>
@@ -1116,13 +1341,16 @@
         <v>49</v>
       </c>
       <c r="D24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" t="s">
         <v>50</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>713777</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-93.27</v>
       </c>
@@ -1133,13 +1361,16 @@
         <v>51</v>
       </c>
       <c r="D25" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" t="s">
         <v>52</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>382578</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-90.18</v>
       </c>
@@ -1150,13 +1381,16 @@
         <v>53</v>
       </c>
       <c r="D26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" t="s">
         <v>54</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>173514</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-94.58</v>
       </c>
@@ -1167,13 +1401,16 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" t="s">
         <v>56</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>459787</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-108.54</v>
       </c>
@@ -1184,13 +1421,16 @@
         <v>57</v>
       </c>
       <c r="D28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" t="s">
         <v>58</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>104170</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-96</v>
       </c>
@@ -1201,13 +1441,16 @@
         <v>59</v>
       </c>
       <c r="D29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" t="s">
         <v>60</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>466893</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-115.14</v>
       </c>
@@ -1218,13 +1461,16 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" t="s">
         <v>62</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>583756</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-71.459999999999994</v>
       </c>
@@ -1235,13 +1481,16 @@
         <v>63</v>
       </c>
       <c r="D31" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" t="s">
         <v>64</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>109565</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-74.17</v>
       </c>
@@ -1252,13 +1501,16 @@
         <v>65</v>
       </c>
       <c r="D32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
         <v>66</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>277140</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-106.61</v>
       </c>
@@ -1269,13 +1521,16 @@
         <v>67</v>
       </c>
       <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
         <v>68</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>545852</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-73.94</v>
       </c>
@@ -1286,13 +1541,16 @@
         <v>69</v>
       </c>
       <c r="D34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" t="s">
         <v>70</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>8175133</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-80.84</v>
       </c>
@@ -1303,13 +1561,16 @@
         <v>71</v>
       </c>
       <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
         <v>72</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>731424</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-96.79</v>
       </c>
@@ -1320,13 +1581,16 @@
         <v>73</v>
       </c>
       <c r="D36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" t="s">
         <v>74</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>105549</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-82.98</v>
       </c>
@@ -1337,13 +1601,16 @@
         <v>75</v>
       </c>
       <c r="D37" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s">
         <v>76</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>879170</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-97.54</v>
       </c>
@@ -1354,13 +1621,16 @@
         <v>77</v>
       </c>
       <c r="D38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
         <v>78</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>579999</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>-122.68</v>
       </c>
@@ -1371,13 +1641,16 @@
         <v>79</v>
       </c>
       <c r="D39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" t="s">
         <v>44</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>583776</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>-75.16</v>
       </c>
@@ -1388,13 +1661,16 @@
         <v>80</v>
       </c>
       <c r="D40" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" t="s">
         <v>81</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>1526006</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>-71.42</v>
       </c>
@@ -1405,13 +1681,16 @@
         <v>82</v>
       </c>
       <c r="D41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" t="s">
         <v>83</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>178042</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-79.930000000000007</v>
       </c>
@@ -1422,13 +1701,16 @@
         <v>84</v>
       </c>
       <c r="D42" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" t="s">
         <v>85</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>129272</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>-96.73</v>
       </c>
@@ -1439,13 +1721,16 @@
         <v>86</v>
       </c>
       <c r="D43" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" t="s">
         <v>87</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>153888</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-86.78</v>
       </c>
@@ -1456,13 +1741,16 @@
         <v>88</v>
       </c>
       <c r="D44" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" t="s">
         <v>89</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>660388</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-95.38</v>
       </c>
@@ -1473,13 +1761,16 @@
         <v>90</v>
       </c>
       <c r="D45" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" t="s">
         <v>91</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>2099451</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-111.88</v>
       </c>
@@ -1490,13 +1781,16 @@
         <v>92</v>
       </c>
       <c r="D46" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" t="s">
         <v>93</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>186440</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-73.209999999999994</v>
       </c>
@@ -1507,13 +1801,16 @@
         <v>94</v>
       </c>
       <c r="D47" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" t="s">
         <v>95</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>42417</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-75.98</v>
       </c>
@@ -1524,13 +1821,16 @@
         <v>96</v>
       </c>
       <c r="D48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" t="s">
         <v>97</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>437994</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-122.33</v>
       </c>
@@ -1541,13 +1841,16 @@
         <v>22</v>
       </c>
       <c r="D49" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" t="s">
         <v>98</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>608660</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-81.63</v>
       </c>
@@ -1558,13 +1861,16 @@
         <v>99</v>
       </c>
       <c r="D50" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" t="s">
         <v>85</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>51400</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-87.95</v>
       </c>
@@ -1575,13 +1881,16 @@
         <v>100</v>
       </c>
       <c r="D51" t="s">
+        <v>154</v>
+      </c>
+      <c r="E51" t="s">
         <v>101</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>594833</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-104.8</v>
       </c>
@@ -1592,14 +1901,17 @@
         <v>102</v>
       </c>
       <c r="D52" t="s">
+        <v>155</v>
+      </c>
+      <c r="E52" t="s">
         <v>103</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>59466</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{6DA01A3F-E4BE-934A-AC34-6DF933618644}"/>
+  <autoFilter ref="A1:F1" xr:uid="{6DA01A3F-E4BE-934A-AC34-6DF933618644}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update usmap_transform() to account for Puerto Rico
</commit_message>
<xml_diff>
--- a/data-raw/citypop.xlsx
+++ b/data-raw/citypop.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
   <si>
     <t>lon</t>
   </si>
@@ -377,6 +377,15 @@
   </si>
   <si>
     <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>San Juan</t>
   </si>
   <si>
     <t>Rhode Island</t>
@@ -511,12 +520,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -529,16 +544,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,13 +570,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -581,6 +596,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -780,17 +796,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -817,10 +833,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1059,12 +1075,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1341,7 +1357,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1368,10 +1384,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1613,7 +1629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2425,10 +2441,10 @@
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="3">
-        <v>-71.42</v>
+        <v>-66.06</v>
       </c>
       <c r="B41" s="3">
-        <v>41.82</v>
+        <v>18.41</v>
       </c>
       <c r="C41" t="s" s="4">
         <v>122</v>
@@ -2440,15 +2456,15 @@
         <v>124</v>
       </c>
       <c r="F41" s="3">
-        <v>178042</v>
+        <v>395326</v>
       </c>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="3">
-        <v>-79.93000000000001</v>
+        <v>-71.42</v>
       </c>
       <c r="B42" s="3">
-        <v>32.78</v>
+        <v>41.82</v>
       </c>
       <c r="C42" t="s" s="4">
         <v>125</v>
@@ -2460,15 +2476,15 @@
         <v>127</v>
       </c>
       <c r="F42" s="3">
-        <v>129272</v>
+        <v>178042</v>
       </c>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="3">
-        <v>-96.73</v>
+        <v>-79.93000000000001</v>
       </c>
       <c r="B43" s="3">
-        <v>43.54</v>
+        <v>32.78</v>
       </c>
       <c r="C43" t="s" s="4">
         <v>128</v>
@@ -2480,15 +2496,15 @@
         <v>130</v>
       </c>
       <c r="F43" s="3">
-        <v>153888</v>
+        <v>129272</v>
       </c>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="3">
-        <v>-86.78</v>
+        <v>-96.73</v>
       </c>
       <c r="B44" s="3">
-        <v>36.17</v>
+        <v>43.54</v>
       </c>
       <c r="C44" t="s" s="4">
         <v>131</v>
@@ -2500,15 +2516,15 @@
         <v>133</v>
       </c>
       <c r="F44" s="3">
-        <v>660388</v>
+        <v>153888</v>
       </c>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="3">
-        <v>-95.38</v>
+        <v>-86.78</v>
       </c>
       <c r="B45" s="3">
-        <v>29.76</v>
+        <v>36.17</v>
       </c>
       <c r="C45" t="s" s="4">
         <v>134</v>
@@ -2520,15 +2536,15 @@
         <v>136</v>
       </c>
       <c r="F45" s="3">
-        <v>2099451</v>
+        <v>660388</v>
       </c>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="3">
-        <v>-111.88</v>
+        <v>-95.38</v>
       </c>
       <c r="B46" s="3">
-        <v>40.75</v>
+        <v>29.76</v>
       </c>
       <c r="C46" t="s" s="4">
         <v>137</v>
@@ -2540,15 +2556,15 @@
         <v>139</v>
       </c>
       <c r="F46" s="3">
-        <v>186440</v>
+        <v>2099451</v>
       </c>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="3">
-        <v>-73.20999999999999</v>
+        <v>-111.88</v>
       </c>
       <c r="B47" s="3">
-        <v>44.48</v>
+        <v>40.75</v>
       </c>
       <c r="C47" t="s" s="4">
         <v>140</v>
@@ -2560,15 +2576,15 @@
         <v>142</v>
       </c>
       <c r="F47" s="3">
-        <v>42417</v>
+        <v>186440</v>
       </c>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="3">
-        <v>-75.98</v>
+        <v>-73.20999999999999</v>
       </c>
       <c r="B48" s="3">
-        <v>36.85</v>
+        <v>44.48</v>
       </c>
       <c r="C48" t="s" s="4">
         <v>143</v>
@@ -2580,75 +2596,75 @@
         <v>145</v>
       </c>
       <c r="F48" s="3">
-        <v>437994</v>
+        <v>42417</v>
       </c>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="3">
-        <v>-122.33</v>
+        <v>-75.98</v>
       </c>
       <c r="B49" s="3">
-        <v>47.61</v>
+        <v>36.85</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="D49" t="s" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E49" t="s" s="4">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F49" s="3">
-        <v>608660</v>
+        <v>437994</v>
       </c>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="3">
-        <v>-81.63</v>
+        <v>-122.33</v>
       </c>
       <c r="B50" s="3">
-        <v>38.35</v>
+        <v>47.61</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>148</v>
+        <v>32</v>
       </c>
       <c r="D50" t="s" s="4">
         <v>149</v>
       </c>
       <c r="E50" t="s" s="4">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="F50" s="3">
-        <v>51400</v>
+        <v>608660</v>
       </c>
     </row>
     <row r="51" ht="15.35" customHeight="1">
       <c r="A51" s="3">
-        <v>-87.95</v>
+        <v>-81.63</v>
       </c>
       <c r="B51" s="3">
-        <v>43.05</v>
+        <v>38.35</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s" s="4">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E51" t="s" s="4">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="F51" s="3">
-        <v>594833</v>
+        <v>51400</v>
       </c>
     </row>
     <row r="52" ht="15.35" customHeight="1">
       <c r="A52" s="3">
-        <v>-104.8</v>
+        <v>-87.95</v>
       </c>
       <c r="B52" s="3">
-        <v>41.15</v>
+        <v>43.05</v>
       </c>
       <c r="C52" t="s" s="4">
         <v>153</v>
@@ -2660,6 +2676,26 @@
         <v>155</v>
       </c>
       <c r="F52" s="3">
+        <v>594833</v>
+      </c>
+    </row>
+    <row r="53" ht="15.35" customHeight="1">
+      <c r="A53" s="3">
+        <v>-104.8</v>
+      </c>
+      <c r="B53" s="3">
+        <v>41.15</v>
+      </c>
+      <c r="C53" t="s" s="4">
+        <v>156</v>
+      </c>
+      <c r="D53" t="s" s="4">
+        <v>157</v>
+      </c>
+      <c r="E53" t="s" s="4">
+        <v>158</v>
+      </c>
+      <c r="F53" s="3">
         <v>59466</v>
       </c>
     </row>

</xml_diff>